<commit_message>
ref #1: implemented logic for parsing TSV file
</commit_message>
<xml_diff>
--- a/webapp/ridlr/master_templates/Quiz-Template.xlsx
+++ b/webapp/ridlr/master_templates/Quiz-Template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Quiz</t>
   </si>
@@ -475,6 +475,9 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="B16" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>